<commit_message>
capturas y TAC para Itsaso
</commit_message>
<xml_diff>
--- a/Capturas_TACs_Itsaso.xlsx
+++ b/Capturas_TACs_Itsaso.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/BOQUERON/BioEcon4Fish/Fcap_ane27.9a_South/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mariajosezunigabasualto/MJZ/BOQUERON/BIOECON4FISH/Fcap/Fcap_ane27.9a_South/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0A64FA0C-345B-AE4C-B096-E128E3038F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A4B6F-641C-7D45-A4E0-7CA944A27CC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17920" yWindow="1020" windowWidth="29400" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="TAC y Capturas 9a" sheetId="1" r:id="rId1"/>
+    <sheet name="Capturas 9a sur" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,20 +40,20 @@
     <author>tc={1A33638A-9FF8-0147-87B0-D3FB0EDED8BE}</author>
   </authors>
   <commentList>
-    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{8DB183F9-0702-6A4D-AAE5-5459B08C1E82}">
+    <comment ref="I34" authorId="0" shapeId="0" xr:uid="{8DB183F9-0702-6A4D-AAE5-5459B08C1E82}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t xml:space="preserve">[Comentario encadenado]
+Tu versión de Excel te permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     Considerando la proporción del segundo semestre por la captura total de un año más la proporción del primer semestre del año siguiente por la captura total del año siguiente
 </t>
       </text>
     </comment>
-    <comment ref="H33" authorId="1" shapeId="0" xr:uid="{1A33638A-9FF8-0147-87B0-D3FB0EDED8BE}">
+    <comment ref="J34" authorId="1" shapeId="0" xr:uid="{1A33638A-9FF8-0147-87B0-D3FB0EDED8BE}">
       <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
+        <t>[Comentario encadenado]
+Tu versión de Excel te permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
     Este viene de la suma de la captura del segundo semestre de un año + la captura del primer semestre del año siguiente</t>
       </text>
     </comment>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
   <si>
     <t>Año</t>
   </si>
@@ -220,20 +220,26 @@
     <t>Semestre 2</t>
   </si>
   <si>
-    <t>Captura años naturales</t>
-  </si>
-  <si>
-    <t>considerando la proporción</t>
-  </si>
-  <si>
     <t>suma de capturas semestrales</t>
+  </si>
+  <si>
+    <t>considerando la proporción semestral</t>
+  </si>
+  <si>
+    <t>Captura año calendario junio-julio y  naturales enero-diciembre</t>
+  </si>
+  <si>
+    <t>Captura aconsejada ICES</t>
+  </si>
+  <si>
+    <t>cambio de modelo y calendario de gestión</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,13 +268,29 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +309,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8766D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00BFC4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF2400"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00F900"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF016400"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0333FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -307,11 +371,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,14 +547,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -338,15 +559,101 @@
     <xf numFmtId="4" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0333FF"/>
+      <color rgb="FF016400"/>
+      <color rgb="FF00F900"/>
+      <color rgb="FFFF2400"/>
+      <color rgb="FF00BFC4"/>
+      <color rgb="FFF8766D"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -356,6 +663,1559 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-MX"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Capturas 9a sur'!$I$2:$I$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>considerando la proporción semestral</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Capturas 9a sur'!$H$4:$H$40</c:f>
+              <c:strCache>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2018–2019</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2019–2020</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2020–2021</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2021–2022</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2022–2023</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2023–2024</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Capturas 9a sur'!$I$4:$I$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>5354.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5819.0640000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5717.3429999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2996.7049999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1959.951</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3035.4569999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>570.61369999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1831.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4613.2129999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9582.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5940.549</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2353.442</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8636.66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8244.2630000000008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4947.8100000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5581.1880000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4440.8202000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4389.0914000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5616.2449999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3219.627</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2954.9209999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2927.4295000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6291.31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4838.2129000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5231.4579999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9046.2350000000006</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6950.09</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6741.8180000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4610.8680000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4498.8140000000003</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="0">
+                  <c:v>3814.9342800000004</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="0">
+                  <c:v>6473.6501000000007</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="0">
+                  <c:v>7890.7290499999999</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="0">
+                  <c:v>6644.1248399999995</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="0">
+                  <c:v>7930.1199100000003</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="0">
+                  <c:v>8053.5367000000006</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5CED-D047-8A40-41524091315E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Capturas 9a sur'!$J$2:$J$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>suma de capturas semestrales</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Capturas 9a sur'!$H$4:$H$40</c:f>
+              <c:strCache>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>1989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2017</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>2018</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2018–2019</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2019–2020</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2020–2021</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2021–2022</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2022–2023</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2023–2024</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2025</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Capturas 9a sur'!$J$4:$J$40</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="0">
+                  <c:v>5354.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5819.0640000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5717.3429999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2996.7049999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1959.951</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3035.4569999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>570.61369999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1831.41</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4613.2129999999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9582.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5940.549</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2353.442</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8636.66</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8244.2630000000008</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4947.8100000000004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5581.1880000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4440.8202000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4389.0914000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5616.2449999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3219.627</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2954.9209999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2927.4295000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6291.31</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4838.2129000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5231.4579999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9046.2350000000006</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>6950.09</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>6741.8180000000002</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4610.8680000000004</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4498.8140000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3814.6289999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6471.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7860.6770000000006</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6631.27</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>7960.4249999999993</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>8071.21</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5CED-D047-8A40-41524091315E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Capturas 9a sur'!$K$2:$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Captura aconsejada ICES</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Capturas 9a sur'!$K$4:$K$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="37"/>
+                <c:pt idx="30">
+                  <c:v>3760</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6290</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>11322</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7181</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1694</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2201</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>7266</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5CED-D047-8A40-41524091315E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1972651120"/>
+        <c:axId val="1973064272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1972651120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1973064272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1973064272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-MX"/>
+                  <a:t>Capturas (t)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-CL"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-CL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1972651120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-CL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-CL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>36287</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90713</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>217714</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>36285</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB92B0A2-F3FC-B9B4-33DD-EBD4E601EAD1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13716001" y="90713"/>
+          <a:ext cx="12264570" cy="8527143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>368300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{929FE842-8A63-A9A5-B010-BAB347B4733F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
@@ -651,11 +2511,11 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="G33" dT="2025-04-15T14:03:15.51" personId="{4088688E-BC5A-B44A-9386-1A03960086B7}" id="{8DB183F9-0702-6A4D-AAE5-5459B08C1E82}">
+  <threadedComment ref="I34" dT="2025-04-15T14:03:15.51" personId="{4088688E-BC5A-B44A-9386-1A03960086B7}" id="{8DB183F9-0702-6A4D-AAE5-5459B08C1E82}">
     <text xml:space="preserve">Considerando la proporción del segundo semestre por la captura total de un año más la proporción del primer semestre del año siguiente por la captura total del año siguiente
 </text>
   </threadedComment>
-  <threadedComment ref="H33" dT="2025-04-15T14:06:17.99" personId="{4088688E-BC5A-B44A-9386-1A03960086B7}" id="{1A33638A-9FF8-0147-87B0-D3FB0EDED8BE}">
+  <threadedComment ref="J34" dT="2025-04-15T14:06:17.99" personId="{4088688E-BC5A-B44A-9386-1A03960086B7}" id="{1A33638A-9FF8-0147-87B0-D3FB0EDED8BE}">
     <text>Este viene de la suma de la captura del segundo semestre de un año + la captura del primer semestre del año siguiente</text>
   </threadedComment>
 </ThreadedComments>
@@ -665,8 +2525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34:F39"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -682,823 +2542,920 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="B2" s="22"/>
+      <c r="C2" s="16">
         <v>4600</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="10">
         <v>5516</v>
       </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="20"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C3">
+      <c r="B3" s="22"/>
+      <c r="C3" s="16">
         <v>6000</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>4173</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="14">
         <v>4721</v>
       </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="20"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="B4" s="22"/>
+      <c r="C4" s="16">
         <v>6000</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="10">
         <v>5259</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="14">
         <v>5944</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <v>5354.25</v>
       </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C5">
+      <c r="B5" s="22"/>
+      <c r="C5" s="16">
         <v>9000</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="10">
         <v>2889</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="14">
         <v>6487</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <v>5819.0640000000003</v>
       </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
+      <c r="B6" s="22"/>
+      <c r="C6" s="16">
         <v>9000</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="10">
         <v>3753</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="14">
         <v>5922</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <v>5717.3430000000008</v>
       </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="B7" s="22"/>
+      <c r="C7" s="16">
         <v>12000</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="10">
         <v>2351</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="14">
         <v>3166</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <v>2996.7049999999999</v>
       </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C8">
+      <c r="B8" s="22"/>
+      <c r="C8" s="16">
         <v>12000</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="10">
         <v>1130</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="14">
         <v>1984</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="12">
         <v>1959.951</v>
       </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="B9" s="22"/>
+      <c r="C9" s="16">
         <v>12000</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="10">
         <v>1619</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="14">
         <v>3388</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <v>3035.4569999999999</v>
       </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10">
+      <c r="B10" s="22"/>
+      <c r="C10" s="16">
         <v>12000</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <v>10106</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="14">
         <v>12956</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="12">
         <v>570.61369999999999</v>
       </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="22"/>
+      <c r="C11" s="16">
         <v>12000</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="10">
         <v>6256</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="14">
         <v>4595</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <v>1831.41</v>
       </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="22"/>
+      <c r="C12" s="16">
         <v>12000</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="10">
         <v>4614</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="14">
         <v>5295</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="12">
         <v>4613.2129999999997</v>
       </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="22"/>
+      <c r="C13" s="16">
         <v>12000</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="10">
         <v>8717</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="14">
         <v>10962</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="12">
         <v>9582.2999999999993</v>
       </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="22">
         <v>4600</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="16">
         <v>13000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="10">
         <v>7486</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="14">
         <v>7409</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="12">
         <v>5940.5490000000009</v>
       </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="22">
         <v>4600</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="16">
         <v>10000</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="10">
         <v>2717</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="14">
         <v>2502</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="12">
         <v>2353.442</v>
       </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="22">
         <v>4900</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="16">
         <v>10000</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="10">
         <v>5907</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="14">
         <v>9098</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="12">
         <v>8636.66</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="G16" s="18"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="22">
         <v>4900</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="16">
         <v>8000</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="10">
         <v>5636</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="14">
         <v>8806</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="12">
         <v>8244.2630000000008</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="G17" s="18"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="22">
         <v>4700</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="16">
         <v>8000</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="10">
         <v>6146</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="14">
         <v>5269</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="12">
         <v>4947.8099999999986</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="G18" s="18"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="22">
         <v>4700</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="16">
         <v>8000</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="10">
         <v>6644</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="14">
         <v>5844</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="12">
         <v>5581.1880000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="G19" s="18"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="22">
         <v>4700</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="16">
         <v>8000</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="10">
         <v>4596</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="14">
         <v>4515</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="12">
         <v>4440.8202000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="G20" s="18"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="22">
         <v>4700</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="16">
         <v>8000</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="10">
         <v>4131</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="14">
         <v>4491</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="12">
         <v>4389.0914000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="G21" s="18"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="22">
         <v>4800</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="16">
         <v>8000</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="10">
         <v>6282</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="14">
         <v>6454</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="12">
         <v>5616.2449999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="G22" s="18"/>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="22">
         <v>4800</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="16">
         <v>8000</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="10">
         <v>3244</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="14">
         <v>3508</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="12">
         <v>3219.627</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="G23" s="18"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="22">
         <v>4800</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="16">
         <v>8000</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="10">
         <v>2349</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="14">
         <v>3013</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="12">
         <v>2954.9209999999998</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="G24" s="18"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="22">
         <v>4800</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="16">
         <v>8000</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="10">
         <v>3291</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="14">
         <v>3210</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="12">
         <v>2927.4295000000002</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="G25" s="18"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C26">
+      <c r="B26" s="22"/>
+      <c r="C26" s="16">
         <v>7600</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="10">
         <v>10134</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="14">
         <v>10076</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="12">
         <v>6291.3099999999986</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="G26" s="18"/>
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C27">
+      <c r="B27" s="22"/>
+      <c r="C27" s="16">
         <v>8600</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="10">
         <v>5589</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="14">
         <v>5589</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="12">
         <v>4838.2129000000004</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="G27" s="18"/>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C28">
+      <c r="B28" s="22"/>
+      <c r="C28" s="16">
         <v>8800</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="10">
         <v>5632</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="14">
         <v>5632</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="12">
         <v>5231.4580000000014</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="G28" s="18"/>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C29">
+      <c r="B29" s="22"/>
+      <c r="C29" s="16">
         <v>8800</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="10">
         <v>7739</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="14">
         <v>10332</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="12">
         <v>9046.2350000000006</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="G29" s="18"/>
+      <c r="H29" s="20"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C30">
+      <c r="B30" s="22"/>
+      <c r="C30" s="16">
         <v>9700</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="10">
         <v>9420</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="14">
         <v>9597</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="12">
         <v>6950.09</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="G30" s="18"/>
+      <c r="H30" s="20"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="22">
         <v>15000</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="16">
         <v>15000</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="10">
         <v>13583</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="14">
         <v>13740</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="12">
         <v>6741.8180000000011</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="G31" s="18"/>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C32">
+      <c r="B32" s="22"/>
+      <c r="C32" s="16">
         <v>12500</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="10">
         <v>13277</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="14">
         <v>14705</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="12">
         <v>4610.8680000000004</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="G32" s="18"/>
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C33">
+      <c r="B33" s="24"/>
+      <c r="C33" s="25">
         <v>12500</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="23">
         <v>13640</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="26">
         <v>13732</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="27">
         <v>4498.8140000000003</v>
       </c>
+      <c r="G33" s="28"/>
+      <c r="H33" s="29"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="A34" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="30">
         <v>17068</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="31">
         <v>17068</v>
       </c>
-      <c r="D34">
-        <v>27510</v>
-      </c>
-      <c r="E34">
-        <v>27814</v>
-      </c>
-      <c r="F34">
+      <c r="D34" s="32">
+        <v>13755</v>
+      </c>
+      <c r="E34" s="33">
+        <v>13907</v>
+      </c>
+      <c r="F34" s="34">
         <v>3814.6289999999999</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="35">
         <v>3760</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="36">
         <v>13308</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="A35" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="22">
         <v>8952</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="16">
         <v>10240</v>
       </c>
-      <c r="D35">
-        <v>18016</v>
-      </c>
-      <c r="E35">
-        <v>18190</v>
-      </c>
-      <c r="F35">
+      <c r="D35" s="10">
+        <v>9008</v>
+      </c>
+      <c r="E35" s="14">
+        <v>9095</v>
+      </c>
+      <c r="F35" s="12">
         <v>6471.7000000000007</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="18">
         <v>6290</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="37">
         <v>2662</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="A36" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="22">
         <v>15669</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="16">
         <v>15669</v>
       </c>
-      <c r="D36">
-        <v>26486</v>
-      </c>
-      <c r="E36">
-        <v>26728</v>
-      </c>
-      <c r="F36">
+      <c r="D36" s="10">
+        <v>13243</v>
+      </c>
+      <c r="E36" s="14">
+        <v>13364</v>
+      </c>
+      <c r="F36" s="12">
         <v>7860.6770000000006</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="18">
         <v>11322</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="37">
         <v>4347</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="A37" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="22">
         <v>15005</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="16">
         <v>15005</v>
       </c>
-      <c r="D37">
-        <v>35700</v>
-      </c>
-      <c r="E37">
-        <v>35962</v>
-      </c>
-      <c r="F37">
+      <c r="D37" s="10">
+        <v>17850</v>
+      </c>
+      <c r="E37" s="14">
+        <v>17981</v>
+      </c>
+      <c r="F37" s="12">
         <v>6631.27</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="18">
         <v>7181</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="37">
         <v>7824</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="A38" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="22">
         <v>15777</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="16">
         <v>15777</v>
       </c>
-      <c r="D38">
-        <v>22028</v>
-      </c>
-      <c r="E38">
-        <v>22462</v>
-      </c>
-      <c r="F38">
+      <c r="D38" s="10">
+        <v>11014</v>
+      </c>
+      <c r="E38" s="14">
+        <v>11231</v>
+      </c>
+      <c r="F38" s="12">
         <v>7960.4249999999993</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="18">
         <v>1694</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="37">
         <v>14083</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="A39" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="22">
         <v>20555</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="16">
         <v>20555</v>
       </c>
-      <c r="D39">
-        <v>20860</v>
-      </c>
-      <c r="E39">
-        <v>20982</v>
-      </c>
-      <c r="F39">
+      <c r="D39" s="10">
+        <v>10430</v>
+      </c>
+      <c r="E39" s="14">
+        <v>10491</v>
+      </c>
+      <c r="F39" s="12">
         <v>8071.21</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="18">
         <v>2201</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="37">
         <v>18354</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="38">
         <v>9449</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="39">
         <v>9449</v>
       </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="G40">
+      <c r="D40" s="40"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="42"/>
+      <c r="G40" s="43">
         <v>969</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="44">
         <v>8480</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3675526-1AB5-7347-9C52-219535AAC8FE}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D2" workbookViewId="0">
+      <selection activeCell="O43" sqref="O43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G1" t="s">
+    <row r="1" spans="1:11" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="55"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="H2" s="53" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="49" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="7"/>
-      <c r="G2" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="K2" s="48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1517,18 +3474,22 @@
       <c r="F3" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H3" s="54"/>
+      <c r="I3" s="49"/>
+      <c r="J3" s="49"/>
+      <c r="K3" s="48"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>1989</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>5354.25</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>3906.59</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>1447.66</v>
       </c>
       <c r="E4" s="3">
@@ -1537,18 +3498,30 @@
       <c r="F4" s="3">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H4" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="50">
+        <f>+B4</f>
+        <v>5354.25</v>
+      </c>
+      <c r="J4" s="50">
+        <f>+B4</f>
+        <v>5354.25</v>
+      </c>
+      <c r="K4" s="10"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>1990</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>5819.0640000000003</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>3871.37</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1947.694</v>
       </c>
       <c r="E5" s="3">
@@ -1557,15 +3530,27 @@
       <c r="F5" s="3">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="50">
+        <f t="shared" ref="I5:I33" si="0">+B5</f>
+        <v>5819.0640000000003</v>
+      </c>
+      <c r="J5" s="50">
+        <f t="shared" ref="J5:J33" si="1">+B5</f>
+        <v>5819.0640000000003</v>
+      </c>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>1991</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>5717.3429999999998</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>4741.8500000000004</v>
       </c>
       <c r="D6" s="3">
@@ -1577,15 +3562,27 @@
       <c r="F6" s="3">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="50">
+        <f t="shared" si="0"/>
+        <v>5717.3429999999998</v>
+      </c>
+      <c r="J6" s="50">
+        <f t="shared" si="1"/>
+        <v>5717.3429999999998</v>
+      </c>
+      <c r="K6" s="10"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>1992</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>2996.7049999999999</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>2493.2800000000002</v>
       </c>
       <c r="D7" s="3">
@@ -1597,15 +3594,27 @@
       <c r="F7" s="3">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="50">
+        <f t="shared" si="0"/>
+        <v>2996.7049999999999</v>
+      </c>
+      <c r="J7" s="50">
+        <f t="shared" si="1"/>
+        <v>2996.7049999999999</v>
+      </c>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>1993</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>1959.951</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>1688.0309999999999</v>
       </c>
       <c r="D8" s="3">
@@ -1617,15 +3626,27 @@
       <c r="F8" s="3">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="50">
+        <f t="shared" si="0"/>
+        <v>1959.951</v>
+      </c>
+      <c r="J8" s="50">
+        <f t="shared" si="1"/>
+        <v>1959.951</v>
+      </c>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>1994</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>3035.4569999999999</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>2744.9450000000002</v>
       </c>
       <c r="D9" s="3">
@@ -1637,8 +3658,20 @@
       <c r="F9" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="50">
+        <f t="shared" si="0"/>
+        <v>3035.4569999999999</v>
+      </c>
+      <c r="J9" s="50">
+        <f t="shared" si="1"/>
+        <v>3035.4569999999999</v>
+      </c>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>1995</v>
       </c>
@@ -1657,12 +3690,24 @@
       <c r="F10" s="3">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="50">
+        <f t="shared" si="0"/>
+        <v>570.61369999999999</v>
+      </c>
+      <c r="J10" s="50">
+        <f t="shared" si="1"/>
+        <v>570.61369999999999</v>
+      </c>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>1996</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>1831.41</v>
       </c>
       <c r="C11" s="3">
@@ -1677,18 +3722,30 @@
       <c r="F11" s="3">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="50">
+        <f t="shared" si="0"/>
+        <v>1831.41</v>
+      </c>
+      <c r="J11" s="50">
+        <f t="shared" si="1"/>
+        <v>1831.41</v>
+      </c>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>1997</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>4613.2129999999997</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>2017.89</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>2595</v>
       </c>
       <c r="E12" s="3">
@@ -1697,18 +3754,30 @@
       <c r="F12" s="3">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="50">
+        <f t="shared" si="0"/>
+        <v>4613.2129999999997</v>
+      </c>
+      <c r="J12" s="50">
+        <f t="shared" si="1"/>
+        <v>4613.2129999999997</v>
+      </c>
+      <c r="K12" s="10"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>1998</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>9582.2999999999993</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>3956.97</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>5625.33</v>
       </c>
       <c r="E13" s="3">
@@ -1717,18 +3786,30 @@
       <c r="F13" s="3">
         <v>0.59</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="50">
+        <f t="shared" si="0"/>
+        <v>9582.2999999999993</v>
+      </c>
+      <c r="J13" s="50">
+        <f t="shared" si="1"/>
+        <v>9582.2999999999993</v>
+      </c>
+      <c r="K13" s="10"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>1999</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>5940.549</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>3633.26</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>2307.2890000000002</v>
       </c>
       <c r="E14" s="3">
@@ -1737,18 +3818,30 @@
       <c r="F14" s="3">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="50">
+        <f t="shared" si="0"/>
+        <v>5940.549</v>
+      </c>
+      <c r="J14" s="50">
+        <f t="shared" si="1"/>
+        <v>5940.549</v>
+      </c>
+      <c r="K14" s="10"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>2000</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>2353.442</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>1080.02</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>1273.422</v>
       </c>
       <c r="E15" s="3">
@@ -1757,18 +3850,30 @@
       <c r="F15" s="3">
         <v>0.54</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="50">
+        <f t="shared" si="0"/>
+        <v>2353.442</v>
+      </c>
+      <c r="J15" s="50">
+        <f t="shared" si="1"/>
+        <v>2353.442</v>
+      </c>
+      <c r="K15" s="10"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>2001</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>8636.66</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>4272.3900000000003</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>4364.2700000000004</v>
       </c>
       <c r="E16" s="3">
@@ -1777,18 +3882,30 @@
       <c r="F16" s="3">
         <v>0.51</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="50">
+        <f t="shared" si="0"/>
+        <v>8636.66</v>
+      </c>
+      <c r="J16" s="50">
+        <f t="shared" si="1"/>
+        <v>8636.66</v>
+      </c>
+      <c r="K16" s="10"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>2002</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>8244.2630000000008</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>4729.2700000000004</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>3514.9929999999999</v>
       </c>
       <c r="E17" s="3">
@@ -1797,18 +3914,30 @@
       <c r="F17" s="3">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H17" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="50">
+        <f t="shared" si="0"/>
+        <v>8244.2630000000008</v>
+      </c>
+      <c r="J17" s="50">
+        <f t="shared" si="1"/>
+        <v>8244.2630000000008</v>
+      </c>
+      <c r="K17" s="10"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>2003</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>4947.8100000000004</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>3566.32</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>1381.49</v>
       </c>
       <c r="E18" s="3">
@@ -1817,18 +3946,30 @@
       <c r="F18" s="3">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H18" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="50">
+        <f t="shared" si="0"/>
+        <v>4947.8100000000004</v>
+      </c>
+      <c r="J18" s="50">
+        <f t="shared" si="1"/>
+        <v>4947.8100000000004</v>
+      </c>
+      <c r="K18" s="10"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>2004</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>5581.1880000000001</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>3360.65</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>2220.538</v>
       </c>
       <c r="E19" s="3">
@@ -1837,15 +3978,27 @@
       <c r="F19" s="3">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="50">
+        <f t="shared" si="0"/>
+        <v>5581.1880000000001</v>
+      </c>
+      <c r="J19" s="50">
+        <f t="shared" si="1"/>
+        <v>5581.1880000000001</v>
+      </c>
+      <c r="K19" s="10"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>2005</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>4440.8202000000001</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>3650.54</v>
       </c>
       <c r="D20" s="3">
@@ -1857,15 +4010,27 @@
       <c r="F20" s="3">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H20" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="I20" s="50">
+        <f t="shared" si="0"/>
+        <v>4440.8202000000001</v>
+      </c>
+      <c r="J20" s="50">
+        <f t="shared" si="1"/>
+        <v>4440.8202000000001</v>
+      </c>
+      <c r="K20" s="10"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>2006</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>4389.0914000000002</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>3954.17</v>
       </c>
       <c r="D21" s="3">
@@ -1877,18 +4042,30 @@
       <c r="F21" s="3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H21" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I21" s="50">
+        <f t="shared" si="0"/>
+        <v>4389.0914000000002</v>
+      </c>
+      <c r="J21" s="50">
+        <f t="shared" si="1"/>
+        <v>4389.0914000000002</v>
+      </c>
+      <c r="K21" s="10"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>2007</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>5616.2449999999999</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>3832.57</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>1783.675</v>
       </c>
       <c r="E22" s="3">
@@ -1897,18 +4074,30 @@
       <c r="F22" s="3">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="50">
+        <f t="shared" si="0"/>
+        <v>5616.2449999999999</v>
+      </c>
+      <c r="J22" s="50">
+        <f t="shared" si="1"/>
+        <v>5616.2449999999999</v>
+      </c>
+      <c r="K22" s="10"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>2008</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>3219.627</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>1733.6369999999999</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>1485.99</v>
       </c>
       <c r="E23" s="3">
@@ -1917,18 +4106,30 @@
       <c r="F23" s="3">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H23" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="50">
+        <f t="shared" si="0"/>
+        <v>3219.627</v>
+      </c>
+      <c r="J23" s="50">
+        <f t="shared" si="1"/>
+        <v>3219.627</v>
+      </c>
+      <c r="K23" s="10"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>2009</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>2954.9209999999998</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>1813.5239999999999</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>1141.3969999999999</v>
       </c>
       <c r="E24" s="3">
@@ -1937,18 +4138,30 @@
       <c r="F24" s="3">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="50">
+        <f t="shared" si="0"/>
+        <v>2954.9209999999998</v>
+      </c>
+      <c r="J24" s="50">
+        <f t="shared" si="1"/>
+        <v>2954.9209999999998</v>
+      </c>
+      <c r="K24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>2010</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>2927.4295000000002</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>1775.5065</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>1151.923</v>
       </c>
       <c r="E25" s="3">
@@ -1957,18 +4170,30 @@
       <c r="F25" s="3">
         <v>0.39</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I25" s="50">
+        <f t="shared" si="0"/>
+        <v>2927.4295000000002</v>
+      </c>
+      <c r="J25" s="50">
+        <f t="shared" si="1"/>
+        <v>2927.4295000000002</v>
+      </c>
+      <c r="K25" s="10"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>2011</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>6291.31</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>3668.75</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>2622.56</v>
       </c>
       <c r="E26" s="3">
@@ -1977,18 +4202,30 @@
       <c r="F26" s="3">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H26" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="I26" s="50">
+        <f t="shared" si="0"/>
+        <v>6291.31</v>
+      </c>
+      <c r="J26" s="50">
+        <f t="shared" si="1"/>
+        <v>6291.31</v>
+      </c>
+      <c r="K26" s="10"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>2012</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>4838.2129000000004</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="4">
         <v>3592.26</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="4">
         <v>1245.9529</v>
       </c>
       <c r="E27" s="3">
@@ -1997,18 +4234,30 @@
       <c r="F27" s="3">
         <v>0.26</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H27" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I27" s="50">
+        <f t="shared" si="0"/>
+        <v>4838.2129000000004</v>
+      </c>
+      <c r="J27" s="50">
+        <f t="shared" si="1"/>
+        <v>4838.2129000000004</v>
+      </c>
+      <c r="K27" s="10"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>2013</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>5231.4579999999996</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="4">
         <v>2271.7359999999999</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="4">
         <v>2959.7220000000002</v>
       </c>
       <c r="E28" s="3">
@@ -2017,18 +4266,30 @@
       <c r="F28" s="3">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="50">
+        <f t="shared" si="0"/>
+        <v>5231.4579999999996</v>
+      </c>
+      <c r="J28" s="50">
+        <f t="shared" si="1"/>
+        <v>5231.4579999999996</v>
+      </c>
+      <c r="K28" s="10"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>2014</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>9046.2350000000006</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="4">
         <v>5307.59</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="4">
         <v>3738.645</v>
       </c>
       <c r="E29" s="3">
@@ -2037,18 +4298,30 @@
       <c r="F29" s="3">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H29" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="50">
+        <f t="shared" si="0"/>
+        <v>9046.2350000000006</v>
+      </c>
+      <c r="J29" s="50">
+        <f t="shared" si="1"/>
+        <v>9046.2350000000006</v>
+      </c>
+      <c r="K29" s="10"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>2015</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>6950.09</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>3895.42</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="4">
         <v>3054.67</v>
       </c>
       <c r="E30" s="3">
@@ -2057,18 +4330,30 @@
       <c r="F30" s="3">
         <v>0.44</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H30" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="50">
+        <f t="shared" si="0"/>
+        <v>6950.09</v>
+      </c>
+      <c r="J30" s="50">
+        <f t="shared" si="1"/>
+        <v>6950.09</v>
+      </c>
+      <c r="K30" s="10"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>2016</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>6741.8180000000002</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>3619.28</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="4">
         <v>3122.538</v>
       </c>
       <c r="E31" s="3">
@@ -2077,18 +4362,30 @@
       <c r="F31" s="3">
         <v>0.46</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="50">
+        <f t="shared" si="0"/>
+        <v>6741.8180000000002</v>
+      </c>
+      <c r="J31" s="50">
+        <f t="shared" si="1"/>
+        <v>6741.8180000000002</v>
+      </c>
+      <c r="K31" s="10"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>2017</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>4610.8680000000004</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="4">
         <v>3264</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="4">
         <v>1346.8679999999999</v>
       </c>
       <c r="E32" s="3">
@@ -2097,204 +4394,283 @@
       <c r="F32" s="3">
         <v>0.28999999999999998</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="8">
+      <c r="H32" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I32" s="50">
+        <f t="shared" si="0"/>
+        <v>4610.8680000000004</v>
+      </c>
+      <c r="J32" s="50">
+        <f t="shared" si="1"/>
+        <v>4610.8680000000004</v>
+      </c>
+      <c r="K32" s="10"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
         <v>2018</v>
       </c>
-      <c r="B33" s="9">
+      <c r="B33" s="7">
         <v>4498.8140000000003</v>
       </c>
-      <c r="C33" s="9">
+      <c r="C33" s="7">
         <v>2627.076</v>
       </c>
-      <c r="D33" s="9">
+      <c r="D33" s="7">
         <v>1871.7380000000001</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="6">
         <v>0.57999999999999996</v>
       </c>
-      <c r="F33" s="8">
+      <c r="F33" s="6">
         <v>0.42</v>
       </c>
-      <c r="G33" s="10">
+      <c r="H33" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I33" s="50">
+        <f t="shared" si="0"/>
+        <v>4498.8140000000003</v>
+      </c>
+      <c r="J33" s="50">
+        <f t="shared" si="1"/>
+        <v>4498.8140000000003</v>
+      </c>
+      <c r="K33" s="10"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B34" s="7">
+        <v>4813.5810000000001</v>
+      </c>
+      <c r="C34" s="7">
+        <v>1942.8910000000001</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2870.69</v>
+      </c>
+      <c r="E34" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="I34" s="51">
         <f>+(B33*F33) +(B34*E34)</f>
         <v>3814.9342800000004</v>
       </c>
-      <c r="H33" s="11">
+      <c r="J34" s="52">
         <f>+D33+C34</f>
         <v>3814.6289999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="8">
-        <v>2019</v>
-      </c>
-      <c r="B34" s="9">
-        <v>4813.5810000000001</v>
-      </c>
-      <c r="C34" s="9">
-        <v>1942.8910000000001</v>
-      </c>
-      <c r="D34" s="9">
-        <v>2870.69</v>
-      </c>
-      <c r="E34" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="F34" s="8">
-        <v>0.6</v>
-      </c>
-      <c r="G34" s="10">
+      <c r="K34" s="10">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B35" s="7">
+        <v>7317.35</v>
+      </c>
+      <c r="C35" s="7">
+        <v>3601.01</v>
+      </c>
+      <c r="D35" s="7">
+        <v>3716.34</v>
+      </c>
+      <c r="E35" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="F35" s="6">
+        <v>0.51</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I35" s="51">
         <f>+(B34*F34) +(B35*E35)</f>
         <v>6473.6501000000007</v>
       </c>
-      <c r="H34" s="11">
+      <c r="J35" s="52">
         <f>+D34+C35</f>
         <v>6471.7000000000007</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="8">
-        <v>2020</v>
-      </c>
-      <c r="B35" s="9">
-        <v>7317.35</v>
-      </c>
-      <c r="C35" s="9">
-        <v>3601.01</v>
-      </c>
-      <c r="D35" s="9">
-        <v>3716.34</v>
-      </c>
-      <c r="E35" s="8">
-        <v>0.49</v>
-      </c>
-      <c r="F35" s="8">
-        <v>0.51</v>
-      </c>
-      <c r="G35" s="10">
+      <c r="K35" s="10">
+        <v>6290</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B36" s="7">
+        <v>7561.6009999999997</v>
+      </c>
+      <c r="C36" s="7">
+        <v>4144.3370000000004</v>
+      </c>
+      <c r="D36" s="7">
+        <v>3417.2640000000001</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="F36" s="6">
+        <v>0.45</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I36" s="51">
         <f>+(B35*F35) +(B36*E36)</f>
         <v>7890.7290499999999</v>
       </c>
-      <c r="H35" s="11">
+      <c r="J36" s="52">
         <f>+D35+C36</f>
         <v>7860.6770000000006</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="8">
-        <v>2021</v>
-      </c>
-      <c r="B36" s="9">
-        <v>7561.6009999999997</v>
-      </c>
-      <c r="C36" s="9">
-        <v>4144.3370000000004</v>
-      </c>
-      <c r="D36" s="9">
-        <v>3417.2640000000001</v>
-      </c>
-      <c r="E36" s="8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="F36" s="8">
-        <v>0.45</v>
-      </c>
-      <c r="G36" s="10">
-        <f t="shared" ref="G36:G37" si="0">+(B36*F36) +(B37*E37)</f>
+      <c r="K36" s="10">
+        <v>11322</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B37" s="7">
+        <v>6615.1109999999999</v>
+      </c>
+      <c r="C37" s="7">
+        <v>3214.0059999999999</v>
+      </c>
+      <c r="D37" s="7">
+        <v>3401.105</v>
+      </c>
+      <c r="E37" s="6">
+        <v>0.49</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0.51</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="51">
+        <f>+(B36*F36) +(B37*E37)</f>
         <v>6644.1248399999995</v>
       </c>
-      <c r="H36" s="11">
+      <c r="J37" s="52">
         <f>+D36+C37</f>
         <v>6631.27</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="8">
-        <v>2022</v>
-      </c>
-      <c r="B37" s="9">
-        <v>6615.1109999999999</v>
-      </c>
-      <c r="C37" s="9">
-        <v>3214.0059999999999</v>
-      </c>
-      <c r="D37" s="9">
-        <v>3401.105</v>
-      </c>
-      <c r="E37" s="8">
-        <v>0.49</v>
-      </c>
-      <c r="F37" s="8">
-        <v>0.51</v>
-      </c>
-      <c r="G37" s="10">
-        <f t="shared" si="0"/>
+      <c r="K37" s="10">
+        <v>7181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B38" s="7">
+        <v>7469.53</v>
+      </c>
+      <c r="C38" s="7">
+        <v>4559.32</v>
+      </c>
+      <c r="D38" s="7">
+        <v>2910.21</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.61</v>
+      </c>
+      <c r="F38" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="I38" s="51">
+        <f>+(B37*F37) +(B38*E38)</f>
         <v>7930.1199100000003</v>
       </c>
-      <c r="H37" s="11">
+      <c r="J38" s="52">
         <f>+D37+C38</f>
         <v>7960.4249999999993</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="8">
-        <v>2023</v>
-      </c>
-      <c r="B38" s="9">
-        <v>7469.53</v>
-      </c>
-      <c r="C38" s="9">
-        <v>4559.32</v>
-      </c>
-      <c r="D38" s="9">
-        <v>2910.21</v>
-      </c>
-      <c r="E38" s="8">
-        <v>0.61</v>
-      </c>
-      <c r="F38" s="8">
-        <v>0.39</v>
-      </c>
-      <c r="G38" s="10">
+      <c r="K38" s="10">
+        <v>1694</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="6">
+        <v>2024</v>
+      </c>
+      <c r="B39" s="7">
+        <v>8291</v>
+      </c>
+      <c r="C39" s="7">
+        <v>5161</v>
+      </c>
+      <c r="D39" s="7">
+        <v>3130</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.62</v>
+      </c>
+      <c r="F39" s="6">
+        <v>0.38</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="I39" s="51">
         <f>+(B38*F38) +(B39*E39)</f>
         <v>8053.5367000000006</v>
       </c>
-      <c r="H38" s="11">
+      <c r="J39" s="52">
         <f>+D38+C39</f>
         <v>8071.21</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="8">
-        <v>2024</v>
-      </c>
-      <c r="B39" s="9">
-        <v>8291</v>
-      </c>
-      <c r="C39" s="9">
-        <v>5161</v>
-      </c>
-      <c r="D39" s="9">
-        <v>3130</v>
-      </c>
-      <c r="E39" s="8">
-        <v>0.62</v>
-      </c>
-      <c r="F39" s="8">
-        <v>0.38</v>
-      </c>
-      <c r="G39" s="10"/>
-      <c r="H39" s="12"/>
-      <c r="I39" s="4"/>
+      <c r="K39" s="10">
+        <v>2201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="H40" s="60">
+        <v>2025</v>
+      </c>
+      <c r="I40" s="57"/>
+      <c r="J40" s="58"/>
+      <c r="K40" s="56">
+        <v>7266</v>
+      </c>
+      <c r="L40" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="M40" s="59"/>
+      <c r="N40" s="59"/>
+      <c r="O40" s="59"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="7">
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="K2:K3"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="J2:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>